<commit_message>
same year tests fix
</commit_message>
<xml_diff>
--- a/tests/functional/same_year/output.xlsx
+++ b/tests/functional/same_year/output.xlsx
@@ -600,7 +600,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="167" zoomScaleNormal="167" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,7 +688,7 @@
         <v>14</v>
       </c>
       <c r="H4" s="3">
-        <v>61.748796550000002</v>
+        <v>61</v>
       </c>
       <c r="I4" s="4">
         <v>0</v>
@@ -720,7 +720,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>

</xml_diff>